<commit_message>
translation check exept iOS
</commit_message>
<xml_diff>
--- a/nodejs/docimg/flow.xlsx
+++ b/nodejs/docimg/flow.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utetsuo/workplace/amazonpay-webviewapp-sample-v2/nodejs/docimg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utetsuo/workplace/amazonpay-sample-app-v2/nodejs/docimg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779468A4-0A0A-674A-9622-4CDEE7203F50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C39613-28C3-174C-8738-4FB308A033C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4720" yWindow="-21140" windowWidth="30140" windowHeight="21120" xr2:uid="{768BDD66-EE21-F447-8F0F-031CD939AA71}"/>
+    <workbookView xWindow="10260" yWindow="-37160" windowWidth="30140" windowHeight="31300" activeTab="1" xr2:uid="{768BDD66-EE21-F447-8F0F-031CD939AA71}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="flow" sheetId="2" r:id="rId1"/>
+    <sheet name="purchase-flow" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -78,6 +79,1946 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>406399</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>777874</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFA7958F-A622-144A-9590-AD92F34231BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4533899" y="457200"/>
+          <a:ext cx="11102975" cy="5194300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>WebView</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>393699</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>809624</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{754FDED0-AB80-8048-B865-EC7CB80E7FFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4521199" y="5940425"/>
+          <a:ext cx="11147425" cy="1641475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Native</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8406BE61-122B-D44E-88EB-88E876B24A70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4508500" y="7874000"/>
+          <a:ext cx="6667500" cy="4953000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Secure WebView</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4A468B1-8FE3-3545-A8A2-98E5FB9B05ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="6632575"/>
+          <a:ext cx="1854200" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Invoke</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Secure WebView</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>746125</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F060BABA-DD98-4C42-BDE7-070C0837F1AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13090525" y="6512560"/>
+          <a:ext cx="1846580" cy="472440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Invoke JavaScript</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> function on WebView</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>15874</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A3A4C52-907A-0840-8FDA-76B1848465BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="18" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6413500" y="7026275"/>
+          <a:ext cx="0" cy="1117599"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>517525</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>88901</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED17FA4C-8083-8640-88E7-439F3B9F8F60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14551025" y="5222240"/>
+          <a:ext cx="61595" cy="1369061"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>118745</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9EDA693-4AF0-514D-9DAE-40D00ACEE610}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6377940" y="5198745"/>
+          <a:ext cx="1028700" cy="927735"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Invoke native app code</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>43180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>55880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE988D43-E1C3-6144-84ED-EB9C82E16F5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9252585" y="7358380"/>
+          <a:ext cx="1760220" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>- Android: App Links</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>- iOS: Universal Links</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>168276</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>777876</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98B4CD2-9703-C946-8CE1-3D1430C7FD6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12550776" y="7867650"/>
+          <a:ext cx="3086100" cy="4953000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Secure WebView</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>73025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85ED7231-66C5-7B4F-9FB9-C81DCFF3489D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10804525" y="6616700"/>
+          <a:ext cx="1854200" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Invoke</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Secure WebView</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>174625</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C3760E8-5576-C54A-A304-4D8EA0319AC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11731625" y="7010400"/>
+          <a:ext cx="1270000" cy="1308100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{101520C8-36D1-4D42-94BD-50176C0497EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14465300" y="7359650"/>
+          <a:ext cx="1765300" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>- Android: Intent</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>- iOS: Custom URL Scheme</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2056130" cy="4138702"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43C58A4B-2FD9-8E45-B873-83AD3EBB2D19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5397500" y="971550"/>
+          <a:ext cx="2056130" cy="4138702"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4A04C55-294D-0842-AC76-A0057C630666}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6413500" y="3190875"/>
+          <a:ext cx="0" cy="3441700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>15874</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2151380" cy="4406122"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC909859-EB5B-A940-93D3-B97638F58891}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5334000" y="8143874"/>
+          <a:ext cx="2151380" cy="4406122"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93C48D94-9D62-034A-8AAF-C7FC33646D03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6842125" y="10379075"/>
+          <a:ext cx="1508125" cy="377825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2169795" cy="4355571"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA2A463D-5379-AE4E-A6C5-EEF547BB7C5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="8223250"/>
+          <a:ext cx="2169795" cy="4355571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>190502</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{877B0482-1775-814D-8FA3-4422F981BB5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="22" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9243060" y="7020560"/>
+          <a:ext cx="9525" cy="3329942"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>98425</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>40640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>301625</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BF99445-56FB-8E49-90E0-7CDB3EF92471}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8328025" y="6543040"/>
+          <a:ext cx="1849120" cy="477520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Invoke JavaScript</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> function on WebView</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2086925" cy="4219575"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7095A37-D7F3-914F-B81B-AEA47401CB71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9128125" y="923925"/>
+          <a:ext cx="2086925" cy="4219575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>63502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>40640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2708E819-FD10-E44D-BAEB-128A3CBAB1FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="22" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9252585" y="5143502"/>
+          <a:ext cx="133350" cy="1399538"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2082800" cy="4316068"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DC579A2-0B56-C142-9AE1-AD7F6694BBAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13053060" y="8310880"/>
+          <a:ext cx="2082800" cy="4316068"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>79377</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>504826</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Arrow Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C244FF1-43C9-4D40-AAB2-9D8DFAC7ABC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14366875" y="6988177"/>
+          <a:ext cx="171451" cy="2578098"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>599440</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2113280" cy="4304541"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EE97DA8-A75A-7040-8306-B4B31985438D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12981940" y="904240"/>
+          <a:ext cx="2113280" cy="4304541"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rounded Rectangle 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85D0F9FC-AFA4-8241-8DF4-D58CC8BFEA92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9255760" y="4409440"/>
+          <a:ext cx="1778000" cy="264160"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Purchase</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>174625</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DA6A8F6-E6FF-5D41-8CE7-F7A316D7964F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="13" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10461625" y="4565650"/>
+          <a:ext cx="1270000" cy="2051050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>353060</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rectangle 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8944094C-992F-DD47-8C60-4156B0ACE8BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11051540" y="5178425"/>
+          <a:ext cx="1028700" cy="927735"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="just"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Invoke native app code</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -132,7 +2073,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Amazon側の画面</a:t>
+            <a:t>The pages on Amazon</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -420,7 +2361,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Amazon側の画面</a:t>
+            <a:t>The pages on Amazon</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -655,61 +2596,6 @@
         <a:xfrm>
           <a:off x="7759700" y="2209800"/>
           <a:ext cx="1333500" cy="158750"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE34796-1EE4-A44F-B65F-4A2FDBA782A8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="11" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10299700" y="2343150"/>
-          <a:ext cx="1295400" cy="1416050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1207,7 +3093,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Amazon側の画面</a:t>
+            <a:t>The pages on Amazon</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1358,7 +3244,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Amazon側の画面</a:t>
+            <a:t>The pages on Amazon</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1817,61 +3703,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D262C398-10AD-2B45-9166-3C805F2F754F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="41" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10414000" y="7829550"/>
-          <a:ext cx="1066800" cy="1416050"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -2086,15 +3917,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:colOff>317500</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>368300</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2109,7 +3940,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1752600" y="482600"/>
+          <a:off x="1968500" y="508000"/>
           <a:ext cx="1701800" cy="596900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2155,7 +3986,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t>カートページ</a:t>
+            <a:t>Cart Page</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2234,7 +4065,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t>購入ページ</a:t>
+            <a:t>Review Page</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2313,8 +4144,37 @@
                 </a:outerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t>Thanksページ</a:t>
+            <a:t>Thanks</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> Page</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2323,15 +4183,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
+      <xdr:colOff>368300</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2346,7 +4206,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1828800" y="5727700"/>
+          <a:off x="2019300" y="5715000"/>
           <a:ext cx="1663700" cy="596900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2392,7 +4252,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t>カートページ</a:t>
+            <a:t>Cart Page</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2471,8 +4331,37 @@
                 </a:outerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t>購入ページ</a:t>
+            <a:t>Reveiw</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> Page</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="6E747A">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2550,7 +4439,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </a:rPr>
-            <a:t>Thanksページ</a:t>
+            <a:t>Thanks Page</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2692,6 +4581,238 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rounded Rectangle 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07C02430-FC1E-5A48-93D6-4C513C37774F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9232900" y="3860800"/>
+          <a:ext cx="1346200" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Purchase</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE34796-1EE4-A44F-B65F-4A2FDBA782A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="11" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10299700" y="2343150"/>
+          <a:ext cx="1295400" cy="1416050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Rounded Rectangle 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D9E26C4-B8F9-BA42-B6B4-EEC0F2895351}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9258300" y="9118600"/>
+          <a:ext cx="1346200" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Purchase</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D262C398-10AD-2B45-9166-3C805F2F754F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="41" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10414000" y="7829550"/>
+          <a:ext cx="1066800" cy="1416050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2993,11 +5114,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96200DD9-C5DC-A34E-AA20-73C6E4D559AE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96EB7A0-F1B0-DA4F-B651-30ECF70371F9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M74" sqref="M74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>